<commit_message>
Termino de la clase de Excel
</commit_message>
<xml_diff>
--- a/Archivos/tablaCursos.xlsx
+++ b/Archivos/tablaCursos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COFFE\Documents\Platzi\UiPath\CursoRPA_Platzi\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0A9D1A-FE91-4CB3-BA3F-296F56815798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EB00FB-C9D8-4113-9F45-557B4782DAC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{8EBCFAE6-6167-4DD9-B9F2-303514F74C7D}"/>
   </bookViews>
@@ -33,60 +33,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+  <si>
+    <t>urlCursos</t>
+  </si>
+  <si>
+    <t>Estatus</t>
+  </si>
+  <si>
+    <t>Curso Avanzado de Creación de RPGs con Unity</t>
+  </si>
+  <si>
+    <t>/clases/rpg-unity/</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Curso de Community Manager</t>
+  </si>
+  <si>
+    <t>/clases/community-manager/</t>
+  </si>
+  <si>
+    <t>Curso de Desarrollo de Videojuegos para Móviles con Unity</t>
+  </si>
+  <si>
+    <t>/clases/movil-unity/</t>
+  </si>
+  <si>
+    <t>Curso de Introducción a la Programación de Videojuegos 3D con Unity</t>
+  </si>
+  <si>
+    <t>/clases/unity-3d/</t>
+  </si>
+  <si>
+    <t>Curso de Programación de Videojuegos 2D con Unity</t>
+  </si>
+  <si>
+    <t>/clases/unity-2d/</t>
+  </si>
+  <si>
+    <t>Curso de Programación de Videojuegos 3D con Unity - 2017</t>
+  </si>
+  <si>
+    <t>/clases/unity-3d-old/</t>
+  </si>
+  <si>
+    <t>Curso de VR con Unity</t>
+  </si>
+  <si>
+    <t>/clases/vr-unity/</t>
+  </si>
   <si>
     <t>cursosEncontrados</t>
   </si>
   <si>
-    <t>urlCursos</t>
-  </si>
-  <si>
-    <t>Estatus</t>
-  </si>
-  <si>
-    <t>Curso Avanzado de Creación de RPGs con Unity</t>
-  </si>
-  <si>
-    <t>/clases/rpg-unity/</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
-    <t>Curso de Community Manager</t>
-  </si>
-  <si>
-    <t>/clases/community-manager/</t>
-  </si>
-  <si>
-    <t>Curso de Desarrollo de Videojuegos para Móviles con Unity</t>
-  </si>
-  <si>
-    <t>/clases/movil-unity/</t>
-  </si>
-  <si>
-    <t>Curso de Introducción a la Programación de Videojuegos 3D con Unity</t>
-  </si>
-  <si>
-    <t>/clases/unity-3d/</t>
-  </si>
-  <si>
-    <t>Curso de Programación de Videojuegos 2D con Unity</t>
-  </si>
-  <si>
-    <t>/clases/unity-2d/</t>
-  </si>
-  <si>
-    <t>Curso de Programación de Videojuegos 3D con Unity - 2017</t>
-  </si>
-  <si>
-    <t>/clases/unity-3d-old/</t>
-  </si>
-  <si>
-    <t>Curso de VR con Unity</t>
-  </si>
-  <si>
-    <t>/clases/vr-unity/</t>
+    <t>Número Curso</t>
   </si>
 </sst>
 </file>
@@ -438,98 +441,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DD5D14-65CF-4423-BC45-E5113D3E4D14}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="65.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>